<commit_message>
Updated the conentents of the results file created.
</commit_message>
<xml_diff>
--- a/output/json_data_to_excel.xlsx
+++ b/output/json_data_to_excel.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="130">
   <si>
     <t>total_calls</t>
   </si>
@@ -75,13 +75,13 @@
     <t>call_lengths.all</t>
   </si>
   <si>
-    <t>['2467fd89-9c6a-4dd2-afe5-f78c6425b8e9', '1369dccb-5d19-498c-96cf-d925cf69c8f9', '11275fbe-bec7-4345-b472-1dc8d9d97f5c']</t>
+    <t>['08e5e78b-62e5-48d7-bb5b-10cb7e86fb61', 'd6ff7423-4637-486b-83dd-7346bfbd6095']</t>
   </si>
   <si>
     <t>[]</t>
   </si>
   <si>
-    <t>[34, 38, 34]</t>
+    <t>[32, 31]</t>
   </si>
   <si>
     <t>Analysis</t>
@@ -183,37 +183,28 @@
     <t>end_at</t>
   </si>
   <si>
-    <t>2467fd89-9c6a-4dd2-afe5-f78c6425b8e9</t>
-  </si>
-  <si>
-    <t>1369dccb-5d19-498c-96cf-d925cf69c8f9</t>
-  </si>
-  <si>
-    <t>11275fbe-bec7-4345-b472-1dc8d9d97f5c</t>
-  </si>
-  <si>
-    <t>mtaD9D8Yajk7BMN5-gen-batch</t>
+    <t>08e5e78b-62e5-48d7-bb5b-10cb7e86fb61</t>
+  </si>
+  <si>
+    <t>d6ff7423-4637-486b-83dd-7346bfbd6095</t>
+  </si>
+  <si>
+    <t>Ijb6MJd9h9CxDp9k-gen-batch</t>
   </si>
   <si>
     <t>17244130489</t>
   </si>
   <si>
-    <t>14126136278</t>
-  </si>
-  <si>
-    <t>+18143389276</t>
-  </si>
-  <si>
-    <t>+12068230969</t>
-  </si>
-  <si>
-    <t>+17209155077</t>
-  </si>
-  <si>
-    <t>2024-08-26T23:33:13.750137+00:00</t>
-  </si>
-  <si>
-    <t>2024-08-26T23:31:01.020062+00:00</t>
+    <t>+18138514882</t>
+  </si>
+  <si>
+    <t>+19122145398</t>
+  </si>
+  <si>
+    <t>2024-08-29T12:52:14.55108+00:00</t>
+  </si>
+  <si>
+    <t>2024-08-29T12:49:56.665805+00:00</t>
   </si>
   <si>
     <t>complete</t>
@@ -222,105 +213,70 @@
     <t>api.prod.bland.ai</t>
   </si>
   <si>
-    <t>{'now': 'Monday, August 26, 2024 7:33 PM', 'now_utc': 'Monday, August 26, 2024 11:33 PM', 'short_from': '8143389276', 'short_to': '7244130489', 'from': '+18143389276', 'to': '+17244130489', 'call_id': '2467fd89-9c6a-4dd2-afe5-f78c6425b8e9', 'phone_number': '+17244130489', 'city': 'WASHINGTON', 'country': 'US', 'state': 'PA', 'zip': '15301', 'language': 'eng', 'office': 'office-2', 'appt_date': 20240827, 'appt_time': '1:00 PM', 'last_name': 'Leisman', 'first_name': 'Ed', 'timestamp': '2024-08-26T19:33:41-04:00', 'timezone': 'America/New_York'}</t>
-  </si>
-  <si>
-    <t>{'now': 'Monday, August 26, 2024 7:31 PM', 'now_utc': 'Monday, August 26, 2024 11:31 PM', 'short_from': '2068230969', 'short_to': '4126136278', 'from': '+12068230969', 'to': '+14126136278', 'call_id': '1369dccb-5d19-498c-96cf-d925cf69c8f9', 'phone_number': '+14126136278', 'city': 'PITTSBURGH', 'country': 'US', 'state': 'PA', 'zip': '15235', 'language': 'eng', 'office': 'office-1', 'last_name': 'van Wyk', 'first_name': 'Johan', 'appt_date': 20240827, 'appt_time': '10:00 AM', 'timestamp': '2024-08-26T19:31:15-04:00', 'timezone': 'America/New_York'}</t>
-  </si>
-  <si>
-    <t>{'now': 'Monday, August 26, 2024 7:31 PM', 'now_utc': 'Monday, August 26, 2024 11:31 PM', 'short_from': '7209155077', 'short_to': '7244130489', 'from': '+17209155077', 'to': '+17244130489', 'call_id': '11275fbe-bec7-4345-b472-1dc8d9d97f5c', 'phone_number': '+17244130489', 'city': 'WASHINGTON', 'country': 'US', 'state': 'PA', 'zip': '15301', 'language': 'eng', 'office': 'office-2', 'last_name': 'Leisman', 'first_name': 'Ed', 'appt_date': 20240827, 'appt_time': '1:00 PM', 'timestamp': '2024-08-26T19:31:36-04:00', 'timezone': 'America/New_York'}</t>
+    <t>{'now': 'Thursday, August 29, 2024 8:52 AM', 'now_utc': 'Thursday, August 29, 2024 12:52 PM', 'short_from': '8138514882', 'short_to': '7244130489', 'from': '+18138514882', 'to': '+17244130489', 'call_id': '08e5e78b-62e5-48d7-bb5b-10cb7e86fb61', 'phone_number': '+17244130489', 'city': 'WASHINGTON', 'country': 'US', 'state': 'PA', 'zip': '15301', 'language': 'eng', 'office': 'office-1', 'appt_date': 20240827, 'appt_time': '9:45 AM', 'last_name': 'Leisman', 'first_name': 'Ed', 'timestamp': '2024-08-29T08:52:47-04:00', 'timezone': 'America/New_York'}</t>
+  </si>
+  <si>
+    <t>{'now': 'Thursday, August 29, 2024 8:50 AM', 'now_utc': 'Thursday, August 29, 2024 12:50 PM', 'short_from': '9122145398', 'short_to': '7244130489', 'from': '+19122145398', 'to': '+17244130489', 'call_id': 'd6ff7423-4637-486b-83dd-7346bfbd6095', 'phone_number': '+17244130489', 'city': 'WASHINGTON', 'country': 'US', 'state': 'PA', 'zip': '15301', 'language': 'eng', 'office': 'office-1', 'last_name': 'Leisman', 'first_name': 'Ed', 'appt_date': 20240827, 'appt_time': '9:45 AM', 'timestamp': '2024-08-29T08:50:35-04:00', 'timezone': 'America/New_York'}</t>
   </si>
   <si>
     <t>voicemail</t>
   </si>
   <si>
-    <t>human</t>
-  </si>
-  <si>
     <t>{}</t>
   </si>
   <si>
-    <t>Summary: The call is an automated confirmation call from Solace Behavioral Health to a patient, reminding them of their appointment scheduled for the next day at 1:00 PM. The patient is not actively engaged in the call, and the system is providing options for the patient to manage their message.</t>
-  </si>
-  <si>
-    <t>Summary: The call was a confirmation call from Solace Behavioral Health to confirm Johan's upcoming appointment scheduled for the next day at 10:00 AM. The health assistant, Jen, verified Johan's availability and confirmed his attendance. The call was brief and to the point, with no issues or concerns raised.</t>
-  </si>
-  <si>
-    <t>Here is a concise and insightful summary of the call:
-The call is a voicemail from Jen, a health assistant at Solace Behavioral Health, confirming an appointment with Ed Leisman for the next day at 1:00 PM. The message is a standard confirmation call, and Jen leaves her name and affiliation to ensure Ed is aware of the upcoming appointment.</t>
-  </si>
-  <si>
-    <t>2024-08-26T23:33:28+00:00</t>
-  </si>
-  <si>
-    <t>2024-08-26T23:31:14+00:00</t>
-  </si>
-  <si>
-    <t>2024-08-26T23:31:24+00:00</t>
+    <t>Summary: The call is an automated confirmation message from Solace Behavioral Health to Ed Lisman, reminding him of his appointment scheduled for the next day at 9:45 AM and requesting him to return the call to 352-678-5550 to confirm.</t>
+  </si>
+  <si>
+    <t>Summary: The call is a series of voicemails between Ed Leisman and Jen from Solace Behavioral Health. Jen is attempting to confirm Ed's appointment scheduled for the next day at 9:45 AM and is requesting that Ed return her call at 352-678-5550.</t>
+  </si>
+  <si>
+    <t>2024-08-29T12:52:37+00:00</t>
+  </si>
+  <si>
+    <t>2024-08-29T12:50:25+00:00</t>
   </si>
   <si>
     <t>ASSISTANT</t>
   </si>
   <si>
-    <t>USER</t>
-  </si>
-  <si>
-    <t xml:space="preserve">user:  I will return your call as soon as possible. 
- agent-action: Wait 
- user:  I will return your call as soon as possible. Thank you. 
- agent-action: Wait 
- assistant: Hello, this is Solace Behavioral Health confirming your appointment tomorrow at 1:00 PM. 
- assistant: Hello, this is Solace Behavioral Health confirming your appointment tomorrow at 1:00 PM. 
- user:  If you are satisfied with your message, 
- user:  press 1. To listen to your message, press 2. To erase and rerecord, press 3. To continue recording where you left off, 
- user:  press 4. 
+    <t>{'last_name': 'string', 'first_name': 'string', 'disposition': 'string', 'rescheduled': 'boolean', 'appointment_time': 'YYYY-MM-DD HH:MM:SS'}</t>
+  </si>
+  <si>
+    <t>{'last_name': 'Leisman', 'first_name': 'Ed', 'disposition': None, 'rescheduled': False, 'appointment_time': '2024-08-30 09:45:00'}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">user:  Hi. This is Ed Lisman. Sorry I missed your call. If you leave your name and number, I will return your call as soon as possible. 
+ user:  Thank you. 
+ assistant: Hello, this is Solace Behavioral Health confirming your appointment tomorrow at 9:45 AM.  Please return our call at 352-678-5550. 
+ assistant: Hello, this is Solace Behavioral Health confirming your appointment tomorrow at 9:45 AM.  Please return our call at 352-678-5550. 
  </t>
   </si>
   <si>
-    <t xml:space="preserve">user:  Hello? 
- assistant: Hello, my name is Jen, I’m a health assistant from Solace Behavioral Health. Is this Johan? 
- user:  Yes. It is. 
- assistant: Hi Johan! I wanted to check in with you about your upcoming appointment at ten o'clock A M tomorrow. I just wanted to confirm if you’ll be able to attend your appointment? Or if it no longer fits your schedule, I wanted to help you find another time. 
- user:  I can make it. 
- assistant: Perfect, thank you. We will see you tomorrow at ten o'clock A M. 
- user:  Thank you very much. 
- assistant: Of course, have a great day! Goodbye. 
+    <t xml:space="preserve">user:  Hi. This is Ed Leisman. Sorry I missed your call. 
+ user:  If you leave your name and number, I will return your call as soon as possible. Thank you. 
+ assistant: Hello, this is Jen from Solace Behavioral Health. 
+ assistant: Hello, this is Solace Behavioral Health confirming your appointment tomorrow at 9:45 AM. Please return our call at 352-678-5550. 
+ assistant: Hello, this is Solace Behavioral Health confirming your appointment tomorrow at 9:45 AM. Please return our call at 352-678-5550. 
  </t>
   </si>
   <si>
-    <t xml:space="preserve">user:  Hi. This is Ed Leisman. Sorry I missed your call. If you leave your name and number, I will return your call as soon as possible. 
- user:  Thank you. 
- assistant: Hello, my name is Jen, I'm a health assistant from Solace Behavioral Health. 
- assistant: Hello, this is Solace Behavioral Health confirming your appointment tomorrow at 1:00 PM. 
- assistant: Hello, this is Solace Behavioral Health confirming your appointment tomorrow at 1:00 PM. 
- user:  If you are satisfied with your message, 
- user:  press 1. To listen to your message, press 2. To erase and rerecord, 
- user:  press 3. To continue recording where you left off, press 4. 
- </t>
-  </si>
-  <si>
-    <t>[{'id': 28931590, 'user': 'user', 'text': ' I will return your call as soon as possible.', 'created_at': '2024-08-26T23:33:35.823498+00:00'}, {'id': 28931594, 'user': 'agent-action', 'text': 'Wait', 'created_at': '2024-08-26T23:33:36.268911+00:00'}, {'id': 28931595, 'user': 'user', 'text': ' I will return your call as soon as possible. Thank you.', 'created_at': '2024-08-26T23:33:36.300202+00:00'}, {'id': 28931596, 'user': 'agent-action', 'text': 'Wait', 'created_at': '2024-08-26T23:33:36.382599+00:00'}, {'id': 28931603, 'user': 'assistant', 'text': 'Hello, this is Solace Behavioral Health confirming your appointment tomorrow at 1:00 PM.', 'created_at': '2024-08-26T23:33:41.357415+00:00'}, {'id': 28931615, 'user': 'assistant', 'text': 'Hello, this is Solace Behavioral Health confirming your appointment tomorrow at 1:00 PM.', 'created_at': '2024-08-26T23:33:46.330056+00:00'}, {'id': 28931639, 'user': 'user', 'text': ' If you are satisfied with your message,', 'created_at': '2024-08-26T23:33:54.89475+00:00'}, {'id': 28931651, 'user': 'user', 'text': ' press 1. To listen to your message, press 2. To erase and rerecord, press 3. To continue recording where you left off,', 'created_at': '2024-08-26T23:33:59.221199+00:00'}, {'id': 28931654, 'user': 'user', 'text': ' press 4.', 'created_at': '2024-08-26T23:34:00.244693+00:00'}]</t>
-  </si>
-  <si>
-    <t>[{'id': 28931351, 'user': 'user', 'text': ' Hello?', 'created_at': '2024-08-26T23:31:17.103133+00:00'}, {'id': 28931355, 'user': 'assistant', 'text': 'Hello, my name is Jen, I’m a health assistant from Solace Behavioral Health. Is this Johan?', 'created_at': '2024-08-26T23:31:21.834248+00:00'}, {'id': 28931359, 'user': 'user', 'text': ' Yes. It is.', 'created_at': '2024-08-26T23:31:24.615212+00:00'}, {'id': 28931370, 'user': 'assistant', 'text': "Hi Johan! I wanted to check in with you about your upcoming appointment at ten o'clock A M tomorrow. I just wanted to confirm if you’ll be able to attend your appointment? Or if it no longer fits your schedule, I wanted to help you find another time.", 'created_at': '2024-08-26T23:31:30.901949+00:00'}, {'id': 28931385, 'user': 'user', 'text': ' I can make it.', 'created_at': '2024-08-26T23:31:40.718196+00:00'}, {'id': 28931391, 'user': 'assistant', 'text': "Perfect, thank you. We will see you tomorrow at ten o'clock A M.", 'created_at': '2024-08-26T23:31:42.823177+00:00'}, {'id': 28931403, 'user': 'user', 'text': ' Thank you very much.', 'created_at': '2024-08-26T23:31:48.344079+00:00'}, {'id': 28931415, 'user': 'assistant', 'text': 'Of course, have a great day! Goodbye.', 'created_at': '2024-08-26T23:31:51.401267+00:00'}]</t>
-  </si>
-  <si>
-    <t>[{'id': 28931372, 'user': 'user', 'text': ' Hi. This is Ed Leisman. Sorry I missed your call. If you leave your name and number, I will return your call as soon as possible.', 'created_at': '2024-08-26T23:31:31.302649+00:00'}, {'id': 28931374, 'user': 'user', 'text': ' Thank you.', 'created_at': '2024-08-26T23:31:31.910002+00:00'}, {'id': 28931377, 'user': 'assistant', 'text': "Hello, my name is Jen, I'm a health assistant from Solace Behavioral Health.", 'created_at': '2024-08-26T23:31:36.118936+00:00'}, {'id': 28931379, 'user': 'assistant', 'text': 'Hello, this is Solace Behavioral Health confirming your appointment tomorrow at 1:00 PM.', 'created_at': '2024-08-26T23:31:36.946025+00:00'}, {'id': 28931389, 'user': 'assistant', 'text': 'Hello, this is Solace Behavioral Health confirming your appointment tomorrow at 1:00 PM.', 'created_at': '2024-08-26T23:31:42.29979+00:00'}, {'id': 28931416, 'user': 'user', 'text': ' If you are satisfied with your message,', 'created_at': '2024-08-26T23:31:51.449979+00:00'}, {'id': 28931421, 'user': 'user', 'text': ' press 1. To listen to your message, press 2. To erase and rerecord,', 'created_at': '2024-08-26T23:31:55.791446+00:00'}, {'id': 28931424, 'user': 'user', 'text': ' press 3. To continue recording where you left off, press 4.', 'created_at': '2024-08-26T23:31:56.853563+00:00'}]</t>
-  </si>
-  <si>
-    <t>34</t>
-  </si>
-  <si>
-    <t>38</t>
-  </si>
-  <si>
-    <t>2024-08-26T23:34:02.000Z</t>
-  </si>
-  <si>
-    <t>2024-08-26T23:31:52.000Z</t>
-  </si>
-  <si>
-    <t>2024-08-26T23:31:58.000Z</t>
+    <t>[{'id': 29548319, 'user': 'user', 'text': ' Hi. This is Ed Lisman. Sorry I missed your call. If you leave your name and number, I will return your call as soon as possible.', 'created_at': '2024-08-29T12:52:44.636017+00:00'}, {'id': 29548326, 'user': 'user', 'text': ' Thank you.', 'created_at': '2024-08-29T12:52:45.247755+00:00'}, {'id': 29548335, 'user': 'assistant', 'text': 'Hello, this is Solace Behavioral Health confirming your appointment tomorrow at 9:45 AM.  Please return our call at 352-678-5550.', 'created_at': '2024-08-29T12:52:47.952466+00:00'}, {'id': 29548366, 'user': 'assistant', 'text': 'Hello, this is Solace Behavioral Health confirming your appointment tomorrow at 9:45 AM.  Please return our call at 352-678-5550.', 'created_at': '2024-08-29T12:52:57.474167+00:00'}]</t>
+  </si>
+  <si>
+    <t>[{'id': 29547749, 'user': 'user', 'text': ' Hi. This is Ed Leisman. Sorry I missed your call.', 'created_at': '2024-08-29T12:50:30.816245+00:00'}, {'id': 29547761, 'user': 'user', 'text': ' If you leave your name and number, I will return your call as soon as possible. Thank you.', 'created_at': '2024-08-29T12:50:33.544009+00:00'}, {'id': 29547768, 'user': 'assistant', 'text': 'Hello, this is Jen from Solace Behavioral Health.', 'created_at': '2024-08-29T12:50:34.82577+00:00'}, {'id': 29547776, 'user': 'assistant', 'text': 'Hello, this is Solace Behavioral Health confirming your appointment tomorrow at 9:45 AM. Please return our call at 352-678-5550.', 'created_at': '2024-08-29T12:50:35.892825+00:00'}, {'id': 29547816, 'user': 'assistant', 'text': 'Hello, this is Solace Behavioral Health confirming your appointment tomorrow at 9:45 AM. Please return our call at 352-678-5550.', 'created_at': '2024-08-29T12:50:45.537329+00:00'}]</t>
+  </si>
+  <si>
+    <t>32</t>
+  </si>
+  <si>
+    <t>31</t>
+  </si>
+  <si>
+    <t>2024-08-29T12:53:09.000Z</t>
+  </si>
+  <si>
+    <t>2024-08-29T12:50:56.000Z</t>
   </si>
   <si>
     <t>Calls</t>
@@ -404,10 +360,25 @@
     <t>call_params.model</t>
   </si>
   <si>
-    <t>2024-08-26T23:26:21.244415+00:00</t>
-  </si>
-  <si>
-    <t>Your name is Jen and you’re a health assistant at Solace Behavioral Health. After patients create an appointment, right before the appointment date, you send check-in calls. Ask them to to confirm their name and whether they'll be able to attend their appointment tomorrow -  if they can't, transfer them to a live person,  and if neither works then ask them for a time that works for them. If a patient misses the appointment, your company loses lots of revenue. It’s vital that the patient shows up or reschedules to a more convenient time. Either works.   Heres an example dialogue Person: Hello? You: Hello, my name is Jen, I’m a health assistant from Solace Behavioral Health. Is this {{first_name}}? Person: Yes this is {{first_name}} You: Hi {{first_name}}! I wanted to check in with you about your upcoming appointment at {{appt_time}} tomorrow. I just wanted to confirm if you’ll be able to attend your appointment? Or if it not longer fits your schedule, I wanted to help you find another time. Person: Gotcha, this was actually the perfect call. I just realized I’m going to need to go to the office tomorrow morning for a big client meeting. I’d love to reschedule to next week if possible? You: (if the person cannot make it) Ok let me transfer you to our scheduling department. Please hold on for a moment while I transfer you. (transfer call)? You: (if the person can make it) Perfect, thank you. We will see you tomorrow at {{appt_time}}. Person: Ok, thank you! You: Of course, have a great day! Goodbye. Person: Goodbye</t>
+    <t>call_params.analysis_schema.first_name</t>
+  </si>
+  <si>
+    <t>call_params.analysis_schema.last_name</t>
+  </si>
+  <si>
+    <t>call_params.analysis_schema.rescheduled</t>
+  </si>
+  <si>
+    <t>call_params.analysis_schema.appointment_time</t>
+  </si>
+  <si>
+    <t>call_params.analysis_schema.disposition</t>
+  </si>
+  <si>
+    <t>2024-08-29T12:49:28.449234+00:00</t>
+  </si>
+  <si>
+    <t>Your name is Jen and you’re a health assistant at Solace Behavioral Health. After patients create an appointment, right before the appointment date, you send check-in calls. Ask them to to confirm their name and whether they'll be able to attend their appointment tomorrow -  if they can't, transfer them to a live person,  and if neither works then ask them for a time that works for them. If a patient misses the appointment, your company loses lots of revenue. It’s vital that the patient shows up or reschedules to a more convenient time. Either works.   Heres an example dialogue Person: Hello? You: Hello, my name is Jen, I’m a health assistant from Solace Behavioral Health. Is this {{first_name}}? Person: Yes this is {{first_name}} You: Hi {{first_name}}! I wanted to check in with you about your upcoming appointment at {{appt_time}} tomorrow. I just wanted to confirm if you’ll be able to attend your appointment? Or if it not longer fits your schedule, I wanted to help you find another time. Person: Gotcha, this was actually the perfect call. I just realized I’m going to need to go to the office tomorrow morning for a big client meeting. I’d love to reschedule to next week if possible? You: (if the person cannot make it) Ok let me transfer you to our scheduling department. Please hold on for a moment while I transfer you. (transfer call)? You: (if the person can make it) Perfect, thank you. We will see you tomorrow at {{appt_time}}. Person: Ok, thank you! You: Of course, have a great day! Goodbye.</t>
   </si>
   <si>
     <t>api</t>
@@ -419,7 +390,10 @@
     <t>leave_message</t>
   </si>
   <si>
-    <t>Hello, this is Solace Behavioral Health confirming your appointment tomorrow at {{appt_time}}.</t>
+    <t>Hello, this is Solace Behavioral Health confirming your appointment tomorrow at {{appt_time}}.  Please return our call at 352-678-5550.</t>
+  </si>
+  <si>
+    <t>Hello, this is Solace Behavioral Health confirming your appointment tomorrow at {{appt_time}}. Please return our call at 352-678-5550.</t>
   </si>
   <si>
     <t>0.6</t>
@@ -429,6 +403,15 @@
   </si>
   <si>
     <t>enhanced</t>
+  </si>
+  <si>
+    <t>string</t>
+  </si>
+  <si>
+    <t>boolean</t>
+  </si>
+  <si>
+    <t>YYYY-MM-DD HH:MM:SS</t>
   </si>
   <si>
     <t>Batch Params</t>
@@ -819,7 +802,7 @@
         <v>0</v>
       </c>
       <c r="B4">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -827,7 +810,7 @@
         <v>1</v>
       </c>
       <c r="B5">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -859,7 +842,7 @@
         <v>5</v>
       </c>
       <c r="B9">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -867,7 +850,7 @@
         <v>6</v>
       </c>
       <c r="B10">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -875,7 +858,7 @@
         <v>7</v>
       </c>
       <c r="B11">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -923,7 +906,7 @@
         <v>13</v>
       </c>
       <c r="B17">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -973,7 +956,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AF6"/>
+  <dimension ref="A1:AF5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -981,7 +964,7 @@
   <sheetData>
     <row r="1" spans="1:32">
       <c r="A1" s="1" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:32">
@@ -1087,40 +1070,40 @@
         <v>55</v>
       </c>
       <c r="B4">
-        <v>0.566666666666667</v>
+        <v>0.533333333333333</v>
       </c>
       <c r="C4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D4" t="s">
         <v>58</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>59</v>
-      </c>
-      <c r="E4" t="s">
-        <v>61</v>
       </c>
       <c r="F4" t="b">
         <v>1</v>
       </c>
       <c r="G4" t="s">
+        <v>61</v>
+      </c>
+      <c r="H4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I4" t="s">
+        <v>63</v>
+      </c>
+      <c r="J4" t="s">
         <v>64</v>
-      </c>
-      <c r="H4" t="b">
-        <v>0</v>
-      </c>
-      <c r="I4" t="s">
-        <v>66</v>
-      </c>
-      <c r="J4" t="s">
-        <v>67</v>
       </c>
       <c r="K4">
         <v>5</v>
       </c>
       <c r="M4" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="N4" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="O4" t="b">
         <v>0</v>
@@ -1129,37 +1112,43 @@
         <v>55</v>
       </c>
       <c r="R4" t="s">
+        <v>68</v>
+      </c>
+      <c r="S4" t="s">
+        <v>69</v>
+      </c>
+      <c r="T4">
+        <v>0.048</v>
+      </c>
+      <c r="U4" t="s">
+        <v>71</v>
+      </c>
+      <c r="V4" t="b">
+        <v>0</v>
+      </c>
+      <c r="W4" t="s">
         <v>73</v>
       </c>
-      <c r="S4" t="s">
+      <c r="Y4" t="s">
         <v>74</v>
       </c>
-      <c r="T4">
-        <v>0.051</v>
-      </c>
-      <c r="U4" t="s">
-        <v>77</v>
-      </c>
-      <c r="V4" t="b">
-        <v>0</v>
-      </c>
-      <c r="W4" t="s">
-        <v>80</v>
+      <c r="Z4" t="s">
+        <v>75</v>
       </c>
       <c r="AB4" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="AC4" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="AD4" t="s">
         <v>28</v>
       </c>
       <c r="AE4" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="AF4" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
     </row>
     <row r="5" spans="1:32">
@@ -1167,40 +1156,40 @@
         <v>56</v>
       </c>
       <c r="B5">
-        <v>0.633333333333333</v>
+        <v>0.5166666666666671</v>
       </c>
       <c r="C5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D5" t="s">
         <v>58</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>60</v>
-      </c>
-      <c r="E5" t="s">
-        <v>62</v>
       </c>
       <c r="F5" t="b">
         <v>1</v>
       </c>
       <c r="G5" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="H5" t="b">
         <v>0</v>
       </c>
       <c r="I5" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="J5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="K5">
         <v>5</v>
       </c>
       <c r="M5" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="N5" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="O5" t="b">
         <v>0</v>
@@ -1209,117 +1198,43 @@
         <v>56</v>
       </c>
       <c r="R5" t="s">
+        <v>68</v>
+      </c>
+      <c r="S5" t="s">
+        <v>70</v>
+      </c>
+      <c r="T5">
+        <v>0.047</v>
+      </c>
+      <c r="U5" t="s">
+        <v>72</v>
+      </c>
+      <c r="V5" t="b">
+        <v>0</v>
+      </c>
+      <c r="W5" t="s">
         <v>73</v>
       </c>
-      <c r="S5" t="s">
+      <c r="Y5" t="s">
+        <v>74</v>
+      </c>
+      <c r="Z5" t="s">
         <v>75</v>
       </c>
-      <c r="T5">
-        <v>0.057</v>
-      </c>
-      <c r="U5" t="s">
-        <v>78</v>
-      </c>
-      <c r="V5" t="b">
-        <v>0</v>
-      </c>
-      <c r="W5" t="s">
-        <v>81</v>
-      </c>
       <c r="AB5" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="AC5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="AD5" t="s">
         <v>28</v>
       </c>
       <c r="AE5" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="AF5" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="6" spans="1:32">
-      <c r="A6" t="s">
-        <v>57</v>
-      </c>
-      <c r="B6">
-        <v>0.566666666666667</v>
-      </c>
-      <c r="C6" t="s">
-        <v>58</v>
-      </c>
-      <c r="D6" t="s">
-        <v>59</v>
-      </c>
-      <c r="E6" t="s">
-        <v>63</v>
-      </c>
-      <c r="F6" t="b">
-        <v>1</v>
-      </c>
-      <c r="G6" t="s">
-        <v>65</v>
-      </c>
-      <c r="H6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I6" t="s">
-        <v>66</v>
-      </c>
-      <c r="J6" t="s">
-        <v>67</v>
-      </c>
-      <c r="K6">
-        <v>5</v>
-      </c>
-      <c r="M6" t="s">
-        <v>70</v>
-      </c>
-      <c r="N6" t="s">
-        <v>71</v>
-      </c>
-      <c r="O6" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>57</v>
-      </c>
-      <c r="R6" t="s">
-        <v>73</v>
-      </c>
-      <c r="S6" t="s">
-        <v>76</v>
-      </c>
-      <c r="T6">
-        <v>0.051</v>
-      </c>
-      <c r="U6" t="s">
-        <v>79</v>
-      </c>
-      <c r="V6" t="b">
-        <v>0</v>
-      </c>
-      <c r="W6" t="s">
-        <v>80</v>
-      </c>
-      <c r="AB6" t="s">
-        <v>84</v>
-      </c>
-      <c r="AC6" t="s">
-        <v>87</v>
-      </c>
-      <c r="AD6" t="s">
-        <v>28</v>
-      </c>
-      <c r="AE6" t="s">
-        <v>88</v>
-      </c>
-      <c r="AF6" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -1329,7 +1244,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B30"/>
+  <dimension ref="A1:B35"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1347,15 +1262,15 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="2" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="B4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="2" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1363,41 +1278,41 @@
         <v>29</v>
       </c>
       <c r="B6" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="2" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="2" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="B8" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="2" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="B9" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="2" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="B10" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="2" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="B11">
         <v>2</v>
@@ -1405,7 +1320,7 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="2" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="B12" t="b">
         <v>0</v>
@@ -1413,7 +1328,7 @@
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="2" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -1421,7 +1336,7 @@
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="2" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="B14">
         <v>60</v>
@@ -1429,23 +1344,23 @@
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="2" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="B15" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="2" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="B16" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="2" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="B17">
         <v>50</v>
@@ -1453,7 +1368,7 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="2" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="B18" t="b">
         <v>0</v>
@@ -1461,44 +1376,44 @@
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="2" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="B19" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="2" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="B20" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="2" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="B21" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="2" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="2" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="B23" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" s="2" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="B24" t="b">
         <v>1</v>
@@ -1506,7 +1421,7 @@
     </row>
     <row r="25" spans="1:2">
       <c r="A25" s="2" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="B25" t="b">
         <v>1</v>
@@ -1514,17 +1429,17 @@
     </row>
     <row r="26" spans="1:2">
       <c r="A26" s="2" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" s="2" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" s="2" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="B28" t="b">
         <v>0</v>
@@ -1532,7 +1447,7 @@
     </row>
     <row r="29" spans="1:2">
       <c r="A29" s="2" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="B29">
         <v>5</v>
@@ -1540,10 +1455,50 @@
     </row>
     <row r="30" spans="1:2">
       <c r="A30" s="2" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="B30" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B31" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="B32" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="B33" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B34" t="s">
         <v>128</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B35" t="s">
+        <v>126</v>
       </c>
     </row>
   </sheetData>

</xml_diff>